<commit_message>
Update number of residential dwellings
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_Demands_BASE.xlsx
+++ b/SuppXLS/Scen_B_SYS_Demands_BASE.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uccireland-my.sharepoint.com/personal/agaur_ucc_ie/Documents/TIM-2.0/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uccireland-my.sharepoint.com/personal/agaur_ucc_ie/Documents/TIM-2.0/TIM/SuppXLS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="87" documentId="13_ncr:1_{A01CDD26-5182-4BC8-9361-792A002E723C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{BDB12956-2080-4EF2-BCA0-CBA5186E14EA}"/>
+  <xr:revisionPtr revIDLastSave="88" documentId="13_ncr:1_{A01CDD26-5182-4BC8-9361-792A002E723C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{BCF2B508-397A-4E5F-ACD6-52DAA556284B}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16330,8 +16330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CL32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20:CL20"/>
+    <sheetView tabSelected="1" topLeftCell="T10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AE26" sqref="AE26:AF28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -22042,10 +22042,10 @@
         <v>492.828423833106</v>
       </c>
       <c r="AE26">
-        <v>502.36472594874499</v>
+        <v>496.36472594874499</v>
       </c>
       <c r="AF26">
-        <v>516.22001380752999</v>
+        <v>514.52001380752995</v>
       </c>
       <c r="AG26">
         <v>530.17405404626902</v>
@@ -22307,7 +22307,7 @@
         <v>1003.43540212397</v>
       </c>
       <c r="AE27">
-        <v>1002.11497030569</v>
+        <v>1003.61497030569</v>
       </c>
       <c r="AF27">
         <v>1009.1830944926101</v>
@@ -22572,10 +22572,10 @@
         <v>877.53441615506995</v>
       </c>
       <c r="AE28">
-        <v>873.21565965240802</v>
+        <v>877.71565965240802</v>
       </c>
       <c r="AF28">
-        <v>876.17112006521802</v>
+        <v>877.87112006521807</v>
       </c>
       <c r="AG28">
         <v>878.89535131181003</v>

</xml_diff>

<commit_message>
Update changed FILL tables
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_Demands_BASE.xlsx
+++ b/SuppXLS/Scen_B_SYS_Demands_BASE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uccireland-my.sharepoint.com/personal/agaur_ucc_ie/Documents/TIM-2.0/TIM/SuppXLS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_TIMES-IE\updates_from_ccr-40a\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="88" documentId="13_ncr:1_{A01CDD26-5182-4BC8-9361-792A002E723C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{BCF2B508-397A-4E5F-ACD6-52DAA556284B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32931668-C00E-4469-9963-02B897A779F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BY-Demands" sheetId="4" r:id="rId1"/>
@@ -1313,7 +1313,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>25400</xdr:colOff>
+          <xdr:colOff>28575</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -1666,21 +1666,21 @@
       <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="6" width="9.08984375" style="1"/>
-    <col min="7" max="7" width="10.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.08984375" style="1"/>
-    <col min="9" max="9" width="11.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.08984375" style="1"/>
+    <col min="1" max="6" width="9.140625" style="1"/>
+    <col min="7" max="7" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="1"/>
+    <col min="9" max="9" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:37" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C4" s="18" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="3:37" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="3:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="19" t="s">
         <v>126</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="6" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>128</v>
       </c>
@@ -1914,7 +1914,7 @@
         <v>0.20769618859639599</v>
       </c>
     </row>
-    <row r="7" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
         <v>128</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>0.47664625412085698</v>
       </c>
     </row>
-    <row r="8" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
         <v>128</v>
       </c>
@@ -2112,7 +2112,7 @@
         <v>0.42809298937083901</v>
       </c>
     </row>
-    <row r="9" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
         <v>128</v>
       </c>
@@ -2211,7 +2211,7 @@
         <v>0.154582741264056</v>
       </c>
     </row>
-    <row r="10" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
         <v>128</v>
       </c>
@@ -2310,7 +2310,7 @@
         <v>9.95787628254481E-2</v>
       </c>
     </row>
-    <row r="11" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
         <v>128</v>
       </c>
@@ -2409,7 +2409,7 @@
         <v>4.5290536808279797E-2</v>
       </c>
     </row>
-    <row r="12" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
         <v>128</v>
       </c>
@@ -2508,7 +2508,7 @@
         <v>0.28082969344526898</v>
       </c>
     </row>
-    <row r="13" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
         <v>128</v>
       </c>
@@ -2607,7 +2607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
         <v>128</v>
       </c>
@@ -2706,7 +2706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="s">
         <v>128</v>
       </c>
@@ -2755,7 +2755,7 @@
       <c r="AJ15" s="26"/>
       <c r="AK15" s="26"/>
     </row>
-    <row r="16" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C16" s="1" t="s">
         <v>128</v>
       </c>
@@ -2804,7 +2804,7 @@
       <c r="AJ16" s="26"/>
       <c r="AK16" s="26"/>
     </row>
-    <row r="17" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
         <v>128</v>
       </c>
@@ -2853,7 +2853,7 @@
       <c r="AJ17" s="26"/>
       <c r="AK17" s="26"/>
     </row>
-    <row r="18" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
         <v>128</v>
       </c>
@@ -2902,7 +2902,7 @@
       <c r="AJ18" s="26"/>
       <c r="AK18" s="26"/>
     </row>
-    <row r="19" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C19" s="1" t="s">
         <v>128</v>
       </c>
@@ -2951,7 +2951,7 @@
       <c r="AJ19" s="26"/>
       <c r="AK19" s="26"/>
     </row>
-    <row r="20" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
         <v>128</v>
       </c>
@@ -3000,7 +3000,7 @@
       <c r="AJ20" s="26"/>
       <c r="AK20" s="26"/>
     </row>
-    <row r="21" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
         <v>128</v>
       </c>
@@ -3049,7 +3049,7 @@
       <c r="AJ21" s="26"/>
       <c r="AK21" s="26"/>
     </row>
-    <row r="22" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
         <v>128</v>
       </c>
@@ -3098,7 +3098,7 @@
       <c r="AJ22" s="26"/>
       <c r="AK22" s="26"/>
     </row>
-    <row r="23" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C23" s="1" t="s">
         <v>128</v>
       </c>
@@ -3147,7 +3147,7 @@
       <c r="AJ23" s="26"/>
       <c r="AK23" s="26"/>
     </row>
-    <row r="24" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C24" s="1" t="s">
         <v>128</v>
       </c>
@@ -3196,7 +3196,7 @@
       <c r="AJ24" s="26"/>
       <c r="AK24" s="26"/>
     </row>
-    <row r="25" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C25" s="1" t="s">
         <v>128</v>
       </c>
@@ -3245,7 +3245,7 @@
       <c r="AJ25" s="26"/>
       <c r="AK25" s="26"/>
     </row>
-    <row r="26" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C26" s="1" t="s">
         <v>128</v>
       </c>
@@ -3294,7 +3294,7 @@
       <c r="AJ26" s="26"/>
       <c r="AK26" s="26"/>
     </row>
-    <row r="27" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C27" s="1" t="s">
         <v>128</v>
       </c>
@@ -3343,7 +3343,7 @@
       <c r="AJ27" s="26"/>
       <c r="AK27" s="26"/>
     </row>
-    <row r="28" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C28" s="1" t="s">
         <v>128</v>
       </c>
@@ -3392,7 +3392,7 @@
       <c r="AJ28" s="26"/>
       <c r="AK28" s="26"/>
     </row>
-    <row r="29" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C29" s="1" t="s">
         <v>128</v>
       </c>
@@ -3441,7 +3441,7 @@
       <c r="AJ29" s="26"/>
       <c r="AK29" s="26"/>
     </row>
-    <row r="30" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C30" s="1" t="s">
         <v>128</v>
       </c>
@@ -3490,7 +3490,7 @@
       <c r="AJ30" s="26"/>
       <c r="AK30" s="26"/>
     </row>
-    <row r="31" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C31" s="1" t="s">
         <v>128</v>
       </c>
@@ -3539,7 +3539,7 @@
       <c r="AJ31" s="26"/>
       <c r="AK31" s="26"/>
     </row>
-    <row r="32" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C32" s="1" t="s">
         <v>128</v>
       </c>
@@ -3588,7 +3588,7 @@
       <c r="AJ32" s="26"/>
       <c r="AK32" s="26"/>
     </row>
-    <row r="33" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C33" s="1" t="s">
         <v>128</v>
       </c>
@@ -3637,7 +3637,7 @@
       <c r="AJ33" s="26"/>
       <c r="AK33" s="26"/>
     </row>
-    <row r="34" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C34" s="1" t="s">
         <v>128</v>
       </c>
@@ -3686,7 +3686,7 @@
       <c r="AJ34" s="26"/>
       <c r="AK34" s="26"/>
     </row>
-    <row r="35" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C35" s="1" t="s">
         <v>128</v>
       </c>
@@ -3735,7 +3735,7 @@
       <c r="AJ35" s="26"/>
       <c r="AK35" s="26"/>
     </row>
-    <row r="36" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C36" s="1" t="s">
         <v>128</v>
       </c>
@@ -3784,7 +3784,7 @@
       <c r="AJ36" s="26"/>
       <c r="AK36" s="26"/>
     </row>
-    <row r="37" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C37" s="1" t="s">
         <v>128</v>
       </c>
@@ -3833,7 +3833,7 @@
       <c r="AJ37" s="26"/>
       <c r="AK37" s="26"/>
     </row>
-    <row r="38" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C38" s="1" t="s">
         <v>128</v>
       </c>
@@ -3856,7 +3856,7 @@
         <v>4.0239683065477196</v>
       </c>
     </row>
-    <row r="39" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C39" s="1" t="s">
         <v>128</v>
       </c>
@@ -3873,7 +3873,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="40" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C40" s="1" t="s">
         <v>128</v>
       </c>
@@ -3890,7 +3890,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="41" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C41" s="1" t="s">
         <v>128</v>
       </c>
@@ -3906,8 +3906,14 @@
       <c r="I41" s="1" t="s">
         <v>141</v>
       </c>
+      <c r="J41" s="1">
+        <v>5.6291760000000002</v>
+      </c>
+      <c r="K41" s="1">
+        <v>5.6291760000000002</v>
+      </c>
     </row>
-    <row r="42" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C42" s="1" t="s">
         <v>128</v>
       </c>
@@ -3922,6 +3928,12 @@
       </c>
       <c r="I42" s="1" t="s">
         <v>143</v>
+      </c>
+      <c r="J42" s="1">
+        <v>0.48</v>
+      </c>
+      <c r="K42" s="1">
+        <v>0.48</v>
       </c>
     </row>
   </sheetData>
@@ -3938,19 +3950,19 @@
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="9.08984375" style="1"/>
-    <col min="4" max="4" width="11.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.08984375" style="1"/>
+    <col min="1" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="2:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="17" t="s">
         <v>123</v>
       </c>
@@ -4071,7 +4083,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="4" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:32" x14ac:dyDescent="0.2">
       <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
@@ -4187,7 +4199,7 @@
         <v>0.15354445783325901</v>
       </c>
     </row>
-    <row r="5" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:32" x14ac:dyDescent="0.2">
       <c r="D5" s="1" t="s">
         <v>8</v>
       </c>
@@ -4303,7 +4315,7 @@
         <v>0.23317216490181936</v>
       </c>
     </row>
-    <row r="6" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:32" x14ac:dyDescent="0.2">
       <c r="D6" s="1" t="s">
         <v>8</v>
       </c>
@@ -4419,7 +4431,7 @@
         <v>0.24823713290628918</v>
       </c>
     </row>
-    <row r="7" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:32" x14ac:dyDescent="0.2">
       <c r="D7" s="1" t="s">
         <v>8</v>
       </c>
@@ -4535,7 +4547,7 @@
         <v>0.26090669324454713</v>
       </c>
     </row>
-    <row r="8" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:32" x14ac:dyDescent="0.2">
       <c r="D8" s="1" t="s">
         <v>8</v>
       </c>
@@ -4651,7 +4663,7 @@
         <v>0.2736127575169699</v>
       </c>
     </row>
-    <row r="9" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:32" x14ac:dyDescent="0.2">
       <c r="D9" s="1" t="s">
         <v>8</v>
       </c>
@@ -4767,7 +4779,7 @@
         <v>0.28751009956239065</v>
       </c>
     </row>
-    <row r="10" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:32" x14ac:dyDescent="0.2">
       <c r="D10" s="1" t="s">
         <v>8</v>
       </c>
@@ -4883,7 +4895,7 @@
         <v>0.30056783714888385</v>
       </c>
     </row>
-    <row r="11" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:32" x14ac:dyDescent="0.2">
       <c r="D11" s="1" t="s">
         <v>8</v>
       </c>
@@ -4999,7 +5011,7 @@
         <v>0.30974736044878864</v>
       </c>
     </row>
-    <row r="12" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:32" x14ac:dyDescent="0.2">
       <c r="D12" s="1" t="s">
         <v>8</v>
       </c>
@@ -5115,7 +5127,7 @@
         <v>0.31809989196694954</v>
       </c>
     </row>
-    <row r="13" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:32" x14ac:dyDescent="0.2">
       <c r="D13" s="1" t="s">
         <v>8</v>
       </c>
@@ -5231,7 +5243,7 @@
         <v>0.32294632822893321</v>
       </c>
     </row>
-    <row r="14" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:32" x14ac:dyDescent="0.2">
       <c r="D14" s="1" t="s">
         <v>8</v>
       </c>
@@ -5347,7 +5359,7 @@
         <v>0.32814797969391801</v>
       </c>
     </row>
-    <row r="15" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:32" x14ac:dyDescent="0.2">
       <c r="D15" s="11" t="s">
         <v>8</v>
       </c>
@@ -5463,7 +5475,7 @@
         <v>0.35260315962707711</v>
       </c>
     </row>
-    <row r="16" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:32" x14ac:dyDescent="0.2">
       <c r="D16" s="1" t="s">
         <v>8</v>
       </c>
@@ -5579,7 +5591,7 @@
         <v>0.53546212748427002</v>
       </c>
     </row>
-    <row r="17" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D17" s="1" t="s">
         <v>8</v>
       </c>
@@ -5695,7 +5707,7 @@
         <v>0.57005767975163846</v>
       </c>
     </row>
-    <row r="18" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D18" s="1" t="s">
         <v>8</v>
       </c>
@@ -5811,7 +5823,7 @@
         <v>0.59915236065349498</v>
       </c>
     </row>
-    <row r="19" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D19" s="1" t="s">
         <v>8</v>
       </c>
@@ -5927,7 +5939,7 @@
         <v>0.62833087006145982</v>
       </c>
     </row>
-    <row r="20" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D20" s="1" t="s">
         <v>8</v>
       </c>
@@ -6043,7 +6055,7 @@
         <v>0.66024505819429835</v>
       </c>
     </row>
-    <row r="21" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D21" s="1" t="s">
         <v>8</v>
       </c>
@@ -6159,7 +6171,7 @@
         <v>0.69023115859843087</v>
       </c>
     </row>
-    <row r="22" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D22" s="1" t="s">
         <v>8</v>
       </c>
@@ -6275,7 +6287,7 @@
         <v>0.71131123510553984</v>
       </c>
     </row>
-    <row r="23" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D23" s="1" t="s">
         <v>8</v>
       </c>
@@ -6391,7 +6403,7 @@
         <v>0.73049218793701065</v>
       </c>
     </row>
-    <row r="24" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D24" s="1" t="s">
         <v>8</v>
       </c>
@@ -6507,7 +6519,7 @@
         <v>0.74162165989886075</v>
       </c>
     </row>
-    <row r="25" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D25" s="1" t="s">
         <v>8</v>
       </c>
@@ -6623,7 +6635,7 @@
         <v>0.75356685653519806</v>
       </c>
     </row>
-    <row r="26" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D26" s="11" t="s">
         <v>8</v>
       </c>
@@ -6739,7 +6751,7 @@
         <v>0.31412261464919838</v>
       </c>
     </row>
-    <row r="27" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D27" s="1" t="s">
         <v>8</v>
       </c>
@@ -6855,7 +6867,7 @@
         <v>0.47702568446146942</v>
       </c>
     </row>
-    <row r="28" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D28" s="1" t="s">
         <v>8</v>
       </c>
@@ -6971,7 +6983,7 @@
         <v>0.50784572971322095</v>
       </c>
     </row>
-    <row r="29" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D29" s="1" t="s">
         <v>8</v>
       </c>
@@ -7087,7 +7099,7 @@
         <v>0.53376522870113652</v>
       </c>
     </row>
-    <row r="30" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D30" s="1" t="s">
         <v>8</v>
       </c>
@@ -7203,7 +7215,7 @@
         <v>0.55975940776155841</v>
       </c>
     </row>
-    <row r="31" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D31" s="1" t="s">
         <v>8</v>
       </c>
@@ -7319,7 +7331,7 @@
         <v>0.58819071346309182</v>
       </c>
     </row>
-    <row r="32" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D32" s="1" t="s">
         <v>8</v>
       </c>
@@ -7435,7 +7447,7 @@
         <v>0.6149043489106939</v>
       </c>
     </row>
-    <row r="33" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D33" s="1" t="s">
         <v>8</v>
       </c>
@@ -7551,7 +7563,7 @@
         <v>0.63368389914993795</v>
       </c>
     </row>
-    <row r="34" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D34" s="1" t="s">
         <v>8</v>
       </c>
@@ -7667,7 +7679,7 @@
         <v>0.65077158226217591</v>
       </c>
     </row>
-    <row r="35" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D35" s="1" t="s">
         <v>8</v>
       </c>
@@ -7783,7 +7795,7 @@
         <v>0.66068646458119173</v>
       </c>
     </row>
-    <row r="36" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D36" s="1" t="s">
         <v>8</v>
       </c>
@@ -7899,7 +7911,7 @@
         <v>0.67132804931519818</v>
       </c>
     </row>
-    <row r="37" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D37" s="11" t="s">
         <v>8</v>
       </c>
@@ -8015,7 +8027,7 @@
         <v>0.15749716055172061</v>
       </c>
     </row>
-    <row r="38" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D38" s="1" t="s">
         <v>8</v>
       </c>
@@ -8131,7 +8143,7 @@
         <v>0.19359234566578742</v>
       </c>
     </row>
-    <row r="39" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D39" s="1" t="s">
         <v>8</v>
       </c>
@@ -8247,7 +8259,7 @@
         <v>0.21374159249605457</v>
       </c>
     </row>
-    <row r="40" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D40" s="1" t="s">
         <v>8</v>
       </c>
@@ -8363,7 +8375,7 @@
         <v>0.23947887504098309</v>
       </c>
     </row>
-    <row r="41" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D41" s="1" t="s">
         <v>8</v>
       </c>
@@ -8479,7 +8491,7 @@
         <v>0.26831526293579661</v>
       </c>
     </row>
-    <row r="42" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D42" s="1" t="s">
         <v>8</v>
       </c>
@@ -8595,7 +8607,7 @@
         <v>0.3006239289874113</v>
       </c>
     </row>
-    <row r="43" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D43" s="1" t="s">
         <v>8</v>
       </c>
@@ -8711,7 +8723,7 @@
         <v>0.33682298088817003</v>
       </c>
     </row>
-    <row r="44" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D44" s="1" t="s">
         <v>8</v>
       </c>
@@ -8827,7 +8839,7 @@
         <v>0.37738087196359965</v>
       </c>
     </row>
-    <row r="45" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D45" s="1" t="s">
         <v>8</v>
       </c>
@@ -8943,7 +8955,7 @@
         <v>0.42282246344494845</v>
       </c>
     </row>
-    <row r="46" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D46" s="1" t="s">
         <v>8</v>
       </c>
@@ -9059,7 +9071,7 @@
         <v>0.47373581671860376</v>
       </c>
     </row>
-    <row r="47" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D47" s="1" t="s">
         <v>8</v>
       </c>
@@ -9175,7 +9187,7 @@
         <v>0.53077980345115405</v>
       </c>
     </row>
-    <row r="48" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D48" s="11" t="s">
         <v>8</v>
       </c>
@@ -9291,7 +9303,7 @@
         <v>0.12806259379618537</v>
       </c>
     </row>
-    <row r="49" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D49" s="1" t="s">
         <v>8</v>
       </c>
@@ -9407,7 +9419,7 @@
         <v>6.4031296898092727E-2</v>
       </c>
     </row>
-    <row r="50" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D50" s="1" t="s">
         <v>8</v>
       </c>
@@ -9523,7 +9535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D51" s="1" t="s">
         <v>8</v>
       </c>
@@ -9639,7 +9651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D52" s="1" t="s">
         <v>8</v>
       </c>
@@ -9755,7 +9767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D53" s="1" t="s">
         <v>8</v>
       </c>
@@ -9871,7 +9883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="54" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D54" s="1" t="s">
         <v>8</v>
       </c>
@@ -9987,7 +9999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="55" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D55" s="1" t="s">
         <v>8</v>
       </c>
@@ -10103,7 +10115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="56" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D56" s="1" t="s">
         <v>8</v>
       </c>
@@ -10219,7 +10231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D57" s="1" t="s">
         <v>8</v>
       </c>
@@ -10335,7 +10347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="58" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D58" s="1" t="s">
         <v>8</v>
       </c>
@@ -10451,7 +10463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="59" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D59" s="11" t="s">
         <v>8</v>
       </c>
@@ -10567,7 +10579,7 @@
         <v>5.6842758875006623E-2</v>
       </c>
     </row>
-    <row r="60" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="60" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D60" s="1" t="s">
         <v>8</v>
       </c>
@@ -10683,7 +10695,7 @@
         <v>6.5911898266037938E-2</v>
       </c>
     </row>
-    <row r="61" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="61" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D61" s="1" t="s">
         <v>8</v>
       </c>
@@ -10799,7 +10811,7 @@
         <v>7.6890053415996307E-2</v>
       </c>
     </row>
-    <row r="62" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="62" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D62" s="1" t="s">
         <v>8</v>
       </c>
@@ -10915,7 +10927,7 @@
         <v>8.8873422743373481E-2</v>
       </c>
     </row>
-    <row r="63" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="63" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D63" s="1" t="s">
         <v>8</v>
       </c>
@@ -11031,7 +11043,7 @@
         <v>0.10129039567850284</v>
       </c>
     </row>
-    <row r="64" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="64" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D64" s="1" t="s">
         <v>8</v>
       </c>
@@ -11147,7 +11159,7 @@
         <v>0.11452848973903919</v>
       </c>
     </row>
-    <row r="65" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="65" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D65" s="1" t="s">
         <v>8</v>
       </c>
@@ -11263,7 +11275,7 @@
         <v>0.12941974829909172</v>
       </c>
     </row>
-    <row r="66" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="66" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D66" s="1" t="s">
         <v>8</v>
       </c>
@@ -11379,7 +11391,7 @@
         <v>0.14719558240697844</v>
       </c>
     </row>
-    <row r="67" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="67" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D67" s="1" t="s">
         <v>8</v>
       </c>
@@ -11495,7 +11507,7 @@
         <v>0.16873211105988936</v>
       </c>
     </row>
-    <row r="68" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="68" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D68" s="1" t="s">
         <v>8</v>
       </c>
@@ -11611,7 +11623,7 @@
         <v>0.17121414759277323</v>
       </c>
     </row>
-    <row r="69" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="69" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D69" s="1" t="s">
         <v>8</v>
       </c>
@@ -11727,7 +11739,7 @@
         <v>0.18442640120500042</v>
       </c>
     </row>
-    <row r="70" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="70" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D70" s="11" t="s">
         <v>8</v>
       </c>
@@ -11843,7 +11855,7 @@
         <v>0.17505912318297531</v>
       </c>
     </row>
-    <row r="71" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="71" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D71" s="1" t="s">
         <v>8</v>
       </c>
@@ -11959,7 +11971,7 @@
         <v>0.11185535316960879</v>
       </c>
     </row>
-    <row r="72" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="72" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D72" s="1" t="s">
         <v>8</v>
       </c>
@@ -12075,7 +12087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="73" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D73" s="1" t="s">
         <v>8</v>
       </c>
@@ -12191,7 +12203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="74" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D74" s="1" t="s">
         <v>8</v>
       </c>
@@ -12307,7 +12319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="75" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D75" s="1" t="s">
         <v>8</v>
       </c>
@@ -12423,7 +12435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="76" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D76" s="1" t="s">
         <v>8</v>
       </c>
@@ -12539,7 +12551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="77" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D77" s="1" t="s">
         <v>8</v>
       </c>
@@ -12655,7 +12667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="78" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D78" s="1" t="s">
         <v>8</v>
       </c>
@@ -12771,7 +12783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="79" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D79" s="1" t="s">
         <v>8</v>
       </c>
@@ -12887,7 +12899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="80" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D80" s="1" t="s">
         <v>8</v>
       </c>
@@ -13003,7 +13015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="81" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D81" s="11" t="s">
         <v>8</v>
       </c>
@@ -13119,7 +13131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="82" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D82" s="1" t="s">
         <v>8</v>
       </c>
@@ -13235,7 +13247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="83" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D83" s="1" t="s">
         <v>8</v>
       </c>
@@ -13351,7 +13363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="84" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D84" s="1" t="s">
         <v>8</v>
       </c>
@@ -13467,7 +13479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="85" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D85" s="1" t="s">
         <v>8</v>
       </c>
@@ -13583,7 +13595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="86" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D86" s="1" t="s">
         <v>8</v>
       </c>
@@ -13699,7 +13711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="87" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D87" s="1" t="s">
         <v>8</v>
       </c>
@@ -13815,7 +13827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="88" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D88" s="1" t="s">
         <v>8</v>
       </c>
@@ -13931,7 +13943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="89" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D89" s="1" t="s">
         <v>8</v>
       </c>
@@ -14047,7 +14059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="90" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D90" s="1" t="s">
         <v>8</v>
       </c>
@@ -14163,7 +14175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="91" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D91" s="1" t="s">
         <v>8</v>
       </c>
@@ -14279,7 +14291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="92" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D92" s="11" t="s">
         <v>8</v>
       </c>
@@ -14395,7 +14407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="93" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D93" s="1" t="s">
         <v>8</v>
       </c>
@@ -14511,7 +14523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="94" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D94" s="1" t="s">
         <v>8</v>
       </c>
@@ -14627,7 +14639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="95" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D95" s="1" t="s">
         <v>8</v>
       </c>
@@ -14743,7 +14755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="96" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D96" s="1" t="s">
         <v>8</v>
       </c>
@@ -14859,7 +14871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="97" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D97" s="1" t="s">
         <v>8</v>
       </c>
@@ -14975,7 +14987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="98" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D98" s="1" t="s">
         <v>8</v>
       </c>
@@ -15091,7 +15103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="99" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D99" s="1" t="s">
         <v>8</v>
       </c>
@@ -15207,7 +15219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="100" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D100" s="1" t="s">
         <v>8</v>
       </c>
@@ -15323,7 +15335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="101" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D101" s="1" t="s">
         <v>8</v>
       </c>
@@ -15439,7 +15451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="102" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D102" s="1" t="s">
         <v>8</v>
       </c>
@@ -15568,40 +15580,38 @@
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.08984375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="3.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="5.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.54296875" style="1" customWidth="1"/>
-    <col min="25" max="25" width="6.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="3.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.5703125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="27" max="28" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="16384" width="9.08984375" style="1"/>
+    <col min="29" max="29" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:30" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" ht="15" x14ac:dyDescent="0.2">
       <c r="C3" s="2" t="str" cm="1">
         <f t="array" ref="C3">INDEX(C5:C7,$A$4)</f>
         <v>IE</v>
@@ -15715,12 +15725,12 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:30" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>62</v>
       </c>
@@ -15835,7 +15845,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>65</v>
       </c>
@@ -15952,7 +15962,7 @@
         <v>*IE-MN</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>66</v>
       </c>
@@ -16069,7 +16079,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>67</v>
       </c>
@@ -16077,7 +16087,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>69</v>
       </c>
@@ -16085,7 +16095,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>71</v>
       </c>
@@ -16093,7 +16103,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>73</v>
       </c>
@@ -16101,7 +16111,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>75</v>
       </c>
@@ -16109,7 +16119,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>77</v>
       </c>
@@ -16117,7 +16127,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>79</v>
       </c>
@@ -16125,7 +16135,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>81</v>
       </c>
@@ -16133,7 +16143,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>83</v>
       </c>
@@ -16141,7 +16151,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>85</v>
       </c>
@@ -16149,7 +16159,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>87</v>
       </c>
@@ -16157,7 +16167,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>89</v>
       </c>
@@ -16165,7 +16175,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>91</v>
       </c>
@@ -16173,7 +16183,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>93</v>
       </c>
@@ -16181,7 +16191,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
         <v>95</v>
       </c>
@@ -16189,7 +16199,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>97</v>
       </c>
@@ -16197,7 +16207,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>99</v>
       </c>
@@ -16205,7 +16215,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>101</v>
       </c>
@@ -16213,7 +16223,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>103</v>
       </c>
@@ -16221,7 +16231,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>105</v>
       </c>
@@ -16229,7 +16239,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
         <v>107</v>
       </c>
@@ -16237,7 +16247,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
         <v>109</v>
       </c>
@@ -16245,7 +16255,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
         <v>111</v>
       </c>
@@ -16253,7 +16263,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
         <v>113</v>
       </c>
@@ -16261,7 +16271,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>115</v>
       </c>
@@ -16269,7 +16279,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
         <v>117</v>
       </c>
@@ -16277,7 +16287,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
         <v>119</v>
       </c>
@@ -16285,7 +16295,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>121</v>
       </c>
@@ -16311,7 +16321,7 @@
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>25400</xdr:colOff>
+                    <xdr:colOff>28575</xdr:colOff>
                     <xdr:row>3</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -16334,15 +16344,15 @@
       <selection activeCell="AE26" sqref="AE26:AF28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="53.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="53.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:90" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -16350,7 +16360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:90" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -16622,7 +16632,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="3" spans="1:90" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:90" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>8</v>
       </c>
@@ -16887,7 +16897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:90" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:90" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>8</v>
       </c>
@@ -17152,7 +17162,7 @@
         <v>43.671154493917797</v>
       </c>
     </row>
-    <row r="5" spans="1:90" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:90" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>8</v>
       </c>
@@ -17417,7 +17427,7 @@
         <v>12.5022203709298</v>
       </c>
     </row>
-    <row r="6" spans="1:90" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:90" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>8</v>
       </c>
@@ -17682,7 +17692,7 @@
         <v>13.257418520759799</v>
       </c>
     </row>
-    <row r="7" spans="1:90" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:90" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -17947,7 +17957,7 @@
         <v>5.7113909867139503</v>
       </c>
     </row>
-    <row r="8" spans="1:90" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:90" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>8</v>
       </c>
@@ -18212,7 +18222,7 @@
         <v>20.756247817050799</v>
       </c>
     </row>
-    <row r="9" spans="1:90" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:90" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>8</v>
       </c>
@@ -18477,7 +18487,7 @@
         <v>1.46491483901718</v>
       </c>
     </row>
-    <row r="10" spans="1:90" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:90" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>8</v>
       </c>
@@ -18741,7 +18751,7 @@
         <v>34.231245841358039</v>
       </c>
     </row>
-    <row r="11" spans="1:90" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:90" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>8</v>
       </c>
@@ -19006,7 +19016,7 @@
         <v>33.121713888304598</v>
       </c>
     </row>
-    <row r="12" spans="1:90" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:90" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>8</v>
       </c>
@@ -19271,7 +19281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:90" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:90" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>8</v>
       </c>
@@ -19536,7 +19546,7 @@
         <v>47.706490867713597</v>
       </c>
     </row>
-    <row r="14" spans="1:90" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:90" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>8</v>
       </c>
@@ -19801,7 +19811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:90" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:90" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>8</v>
       </c>
@@ -20066,7 +20076,7 @@
         <v>4.10614807311799</v>
       </c>
     </row>
-    <row r="16" spans="1:90" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:90" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>8</v>
       </c>
@@ -20331,7 +20341,7 @@
         <v>12.8068170814614</v>
       </c>
     </row>
-    <row r="17" spans="2:90" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:90" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>8</v>
       </c>
@@ -20452,7 +20462,7 @@
         <v>26.281462653597</v>
       </c>
     </row>
-    <row r="18" spans="2:90" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:90" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>8</v>
       </c>
@@ -20573,7 +20583,7 @@
         <v>56.505144705233697</v>
       </c>
     </row>
-    <row r="19" spans="2:90" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:90" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>8</v>
       </c>
@@ -20694,7 +20704,7 @@
         <v>48.620705909154502</v>
       </c>
     </row>
-    <row r="20" spans="2:90" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:90" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>8</v>
       </c>
@@ -20958,7 +20968,7 @@
         <v>78.363764134641542</v>
       </c>
     </row>
-    <row r="21" spans="2:90" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:90" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>8</v>
       </c>
@@ -21065,7 +21075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:90" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:90" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>8</v>
       </c>
@@ -21330,7 +21340,7 @@
         <v>20.455860184034901</v>
       </c>
     </row>
-    <row r="23" spans="2:90" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:90" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>8</v>
       </c>
@@ -21427,7 +21437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:90" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:90" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>8</v>
       </c>
@@ -21692,7 +21702,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="25" spans="2:90" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:90" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>8</v>
       </c>
@@ -21957,7 +21967,7 @@
         <v>74.697245960000004</v>
       </c>
     </row>
-    <row r="26" spans="2:90" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:90" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>8</v>
       </c>
@@ -22222,7 +22232,7 @@
         <v>1525.3321304907599</v>
       </c>
     </row>
-    <row r="27" spans="2:90" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:90" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>8</v>
       </c>
@@ -22487,7 +22497,7 @@
         <v>1254.2955320809799</v>
       </c>
     </row>
-    <row r="28" spans="2:90" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:90" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>8</v>
       </c>
@@ -22752,7 +22762,7 @@
         <v>814.43878355607001</v>
       </c>
     </row>
-    <row r="29" spans="2:90" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:90" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>8</v>
       </c>
@@ -23016,7 +23026,7 @@
         <v>74.050423599120023</v>
       </c>
     </row>
-    <row r="30" spans="2:90" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:90" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>8</v>
       </c>
@@ -23280,7 +23290,7 @@
         <v>148.99302097654268</v>
       </c>
     </row>
-    <row r="31" spans="2:90" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:90" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>8</v>
       </c>
@@ -23325,7 +23335,7 @@
         <v>40.299999999999997</v>
       </c>
     </row>
-    <row r="32" spans="2:90" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:90" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>8</v>
       </c>

</xml_diff>